<commit_message>
Creacion de reporte de indicadores
</commit_message>
<xml_diff>
--- a/public/reportes/mirBD.xlsx
+++ b/public/reportes/mirBD.xlsx
@@ -183,6 +183,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="J2" s="0" t="inlineStr">
+        <is>
+          <t>aaaa</t>
+        </is>
+      </c>
       <c r="K2" s="0" t="inlineStr">
         <is>
           <t>Area 2</t>
@@ -232,6 +237,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="J3" s="0" t="inlineStr">
+        <is>
+          <t>aasdfdfgh</t>
+        </is>
+      </c>
       <c r="K3" s="0" t="inlineStr">
         <is>
           <t>Area 1 de la Dependencia Admin </t>
@@ -281,6 +291,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="J4" s="0" t="inlineStr">
+        <is>
+          <t>aasdfdfgh</t>
+        </is>
+      </c>
       <c r="K4" s="0" t="inlineStr">
         <is>
           <t>Area 1 de la Dependencia Admin </t>
@@ -330,6 +345,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="J5" s="0" t="inlineStr">
+        <is>
+          <t>aaa</t>
+        </is>
+      </c>
       <c r="K5" s="0" t="inlineStr">
         <is>
           <t>Area 2 de la Dependencia Admin </t>
@@ -379,6 +399,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="J6" s="0" t="inlineStr">
+        <is>
+          <t>Este es un supuesto</t>
+        </is>
+      </c>
       <c r="K6" s="0" t="inlineStr">
         <is>
           <t>Area 2</t>
@@ -428,6 +453,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="J7" s="0" t="inlineStr">
+        <is>
+          <t>aa</t>
+        </is>
+      </c>
       <c r="K7" s="0" t="inlineStr">
         <is>
           <t>Area 2 de la Dependencia Admin </t>
@@ -451,30 +481,35 @@
       </c>
       <c r="D8" s="0" t="inlineStr">
         <is>
-          <t>Estrategia</t>
+          <t>Componente</t>
         </is>
       </c>
       <c r="E8" s="0">
-        <v>5990</v>
+        <v>5529</v>
       </c>
       <c r="F8" s="0" t="inlineStr">
         <is>
-          <t>Programa Presupuestario 101</t>
+          <t>Programa Presupuestario 3</t>
         </is>
       </c>
       <c r="G8" s="0" t="inlineStr">
         <is>
-          <t>aa</t>
+          <t>Optimizar la generación de recursos propios estatales </t>
         </is>
       </c>
       <c r="H8" s="0" t="inlineStr">
         <is>
-          <t>aaa</t>
+          <t>Subasta pública electrónica</t>
         </is>
       </c>
       <c r="I8" s="0" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J8" s="0" t="inlineStr">
+        <is>
+          <t>Supuesto de la actividad Aprovechar los recursos propios</t>
         </is>
       </c>
       <c r="K8" s="0" t="inlineStr">
@@ -492,7 +527,7 @@
       </c>
       <c r="B9" s="0" t="inlineStr">
         <is>
-          <t>Admin </t>
+          <t>Secretaría de Finanzas</t>
         </is>
       </c>
       <c r="C9" s="0">
@@ -500,25 +535,25 @@
       </c>
       <c r="D9" s="0" t="inlineStr">
         <is>
-          <t>Propósito</t>
+          <t>Estrategia</t>
         </is>
       </c>
       <c r="E9" s="0">
-        <v>5995</v>
+        <v>5990</v>
       </c>
       <c r="F9" s="0" t="inlineStr">
         <is>
-          <t>Programa Presupuestario 1</t>
+          <t>Programa Presupuestario 101</t>
         </is>
       </c>
       <c r="G9" s="0" t="inlineStr">
         <is>
-          <t>aaa</t>
+          <t>aa</t>
         </is>
       </c>
       <c r="H9" s="0" t="inlineStr">
         <is>
-          <t>aaaa</t>
+          <t>aaa</t>
         </is>
       </c>
       <c r="I9" s="0" t="inlineStr">
@@ -526,9 +561,14 @@
           <t>1</t>
         </is>
       </c>
+      <c r="J9" s="0" t="inlineStr">
+        <is>
+          <t>qqqq</t>
+        </is>
+      </c>
       <c r="K9" s="0" t="inlineStr">
         <is>
-          <t>Area 1 de la Dependencia Admin </t>
+          <t>Area 1</t>
         </is>
       </c>
     </row>
@@ -553,31 +593,36 @@
         </is>
       </c>
       <c r="E10" s="0">
-        <v>5992</v>
+        <v>5995</v>
       </c>
       <c r="F10" s="0" t="inlineStr">
         <is>
-          <t>Programa Presupuestario 12</t>
+          <t>Programa Presupuestario 1</t>
         </is>
       </c>
       <c r="G10" s="0" t="inlineStr">
         <is>
-          <t>ddd</t>
+          <t>aaa</t>
         </is>
       </c>
       <c r="H10" s="0" t="inlineStr">
         <is>
-          <t>gg</t>
+          <t>aaaa</t>
         </is>
       </c>
       <c r="I10" s="0" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J10" s="0" t="inlineStr">
+        <is>
+          <t>aaaaaa</t>
         </is>
       </c>
       <c r="K10" s="0" t="inlineStr">
         <is>
-          <t>Area 2 de la Dependencia Admin </t>
+          <t>Area 1 de la Dependencia Admin </t>
         </is>
       </c>
     </row>
@@ -590,7 +635,7 @@
       </c>
       <c r="B11" s="0" t="inlineStr">
         <is>
-          <t>Secretaría de Finanzas</t>
+          <t>Admin </t>
         </is>
       </c>
       <c r="C11" s="0">
@@ -602,21 +647,21 @@
         </is>
       </c>
       <c r="E11" s="0">
-        <v>5993</v>
+        <v>5992</v>
       </c>
       <c r="F11" s="0" t="inlineStr">
         <is>
-          <t>Programa Presupuestario 4</t>
+          <t>Programa Presupuestario 12</t>
         </is>
       </c>
       <c r="G11" s="0" t="inlineStr">
         <is>
-          <t>aaaaaa</t>
+          <t>ddd</t>
         </is>
       </c>
       <c r="H11" s="0" t="inlineStr">
         <is>
-          <t>aaa</t>
+          <t>gg</t>
         </is>
       </c>
       <c r="I11" s="0" t="inlineStr">
@@ -624,9 +669,14 @@
           <t>2</t>
         </is>
       </c>
+      <c r="J11" s="0" t="inlineStr">
+        <is>
+          <t>ggg</t>
+        </is>
+      </c>
       <c r="K11" s="0" t="inlineStr">
         <is>
-          <t>Area 1 de la Dependencia Secretaría de Finanzas</t>
+          <t>Area 2 de la Dependencia Admin </t>
         </is>
       </c>
     </row>
@@ -651,29 +701,88 @@
         </is>
       </c>
       <c r="E12" s="0">
+        <v>5993</v>
+      </c>
+      <c r="F12" s="0" t="inlineStr">
+        <is>
+          <t>Programa Presupuestario 4</t>
+        </is>
+      </c>
+      <c r="G12" s="0" t="inlineStr">
+        <is>
+          <t>aaaaaa</t>
+        </is>
+      </c>
+      <c r="H12" s="0" t="inlineStr">
+        <is>
+          <t>aaa</t>
+        </is>
+      </c>
+      <c r="I12" s="0" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J12" s="0" t="inlineStr">
+        <is>
+          <t>TEst TEst TEst TEst TEst TEst TEst TEst TEst TEst TEst TEst TEst TEst TEst TEst TEst TEst TEst TEst TEst TEst TEst TEst TEst TEst vv</t>
+        </is>
+      </c>
+      <c r="K12" s="0" t="inlineStr">
+        <is>
+          <t>Area 1 de la Dependencia Secretaría de Finanzas</t>
+        </is>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>Gobierno Ciudadano
+</t>
+        </is>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>Secretaría de Finanzas</t>
+        </is>
+      </c>
+      <c r="C13" s="0">
+        <v>2022</v>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>Propósito</t>
+        </is>
+      </c>
+      <c r="E13" s="0">
         <v>5991</v>
       </c>
-      <c r="F12" s="0" t="inlineStr">
+      <c r="F13" s="0" t="inlineStr">
         <is>
           <t>Programa Presupuestario 7</t>
         </is>
       </c>
-      <c r="G12" s="0" t="inlineStr">
-        <is>
-          <t>aaa</t>
-        </is>
-      </c>
-      <c r="H12" s="0" t="inlineStr">
+      <c r="G13" s="0" t="inlineStr">
+        <is>
+          <t>aaa</t>
+        </is>
+      </c>
+      <c r="H13" s="0" t="inlineStr">
         <is>
           <t>ggg</t>
         </is>
       </c>
-      <c r="I12" s="0" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K12" s="0" t="inlineStr">
+      <c r="I13" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J13" s="0" t="inlineStr">
+        <is>
+          <t>aaaa</t>
+        </is>
+      </c>
+      <c r="K13" s="0" t="inlineStr">
         <is>
           <t>Area 2</t>
         </is>

</xml_diff>

<commit_message>
Version de git con reportes
</commit_message>
<xml_diff>
--- a/public/reportes/mirBD.xlsx
+++ b/public/reportes/mirBD.xlsx
@@ -14,7 +14,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -43,8 +43,13 @@
       <b/>
       <i/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -61,6 +66,11 @@
         <fgColor rgb="FFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9A8"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -73,7 +83,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyBorder="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyBorder="0"/>
@@ -81,6 +91,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyBorder="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyBorder="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -97,6 +108,11 @@
           <t>Organismo</t>
         </is>
       </c>
+      <c r="B1" s="0" t="inlineStr">
+        <is>
+          <t>Secretaría de Finanzas</t>
+        </is>
+      </c>
       <c r="H1" s="2" t="inlineStr">
         <is>
           <t>REPORTE MIR</t>
@@ -183,7 +199,7 @@
       </c>
       <c r="B10" s="0" t="inlineStr">
         <is>
-          <t>07-19-2022 12:52:25 pm</t>
+          <t>09-19-2022 02:24:36 pm</t>
         </is>
       </c>
     </row>
@@ -225,100 +241,101 @@
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="0" t="inlineStr">
-        <is>
-          <t>Actividad</t>
-        </is>
-      </c>
-      <c r="B12" s="0">
-        <v>4974</v>
-      </c>
-      <c r="C12" s="0" t="inlineStr">
-        <is>
-          <t>6.1.4.2 Avanzar en la digitalización de trámites y servicios.</t>
-        </is>
-      </c>
-      <c r="D12" s="0" t="inlineStr">
-        <is>
-          <t>Porcentaje de etapas concluidas del aplicativo web para el arrendamiento de inmuebles con respecto al total de etapas propuestas para el portal web para el arrendamiento de inmuebles</t>
-        </is>
-      </c>
-      <c r="E12" s="0" t="inlineStr">
-        <is>
-          <t>Bitácora digital de avances del proyecto</t>
-        </is>
-      </c>
-      <c r="F12" s="0" t="inlineStr">
-        <is>
-          <t>Proporcionar una plataforma web del AJOD y del Estadio Corregidora para el mes de diciembre del presente.</t>
-        </is>
-      </c>
-      <c r="G12" s="0" t="inlineStr">
-        <is>
-          <t>Oficialía Mayor</t>
+      <c r="A12" s="5" t="inlineStr">
+        <is>
+          <t>Componente</t>
+        </is>
+      </c>
+      <c r="B12" s="5">
+        <v>5522</v>
+      </c>
+      <c r="C12" s="5" t="inlineStr">
+        <is>
+          <t>1 Salud y Vida Digna</t>
+        </is>
+      </c>
+      <c r="D12" s="5" t="inlineStr">
+        <is>
+          <t>Calificación crediticia de la Entidad | Calificación crediticia de la Entidad | Calificación crediticia de la Entidad</t>
+        </is>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5" t="inlineStr">
+        <is>
+          <t>Supuesto</t>
+        </is>
+      </c>
+      <c r="G12" s="5" t="inlineStr">
+        <is>
+          <t>Secretaría de Finanzas</t>
         </is>
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="0" t="inlineStr">
-        <is>
-          <t>Actividad</t>
-        </is>
-      </c>
-      <c r="B13" s="0">
-        <v>4976</v>
-      </c>
-      <c r="C13" s="0" t="inlineStr">
-        <is>
-          <t>6.1.4.2 Avanzar en la digitalización de trámites y servicios.</t>
-        </is>
-      </c>
-      <c r="D13" s="0" t="inlineStr">
-        <is>
-          <t>Porcentaje de etapas concluidas de la implentación de la plataforma digital con Total de etapas para la implementación de la plataforma digital</t>
-        </is>
-      </c>
-      <c r="E13" s="0" t="inlineStr">
-        <is>
-          <t>Bitácora digital de avances del proyecto</t>
-        </is>
-      </c>
-      <c r="F13" s="0" t="inlineStr">
-        <is>
-          <t>Cumplir para el mes de noviembre con las adecuaciones solicitadas por la Dirección de Adquisiciones</t>
-        </is>
-      </c>
-      <c r="G13" s="0" t="inlineStr">
-        <is>
-          <t>Oficialía Mayor</t>
+      <c r="A13" s="5" t="inlineStr">
+        <is>
+          <t>Componente</t>
+        </is>
+      </c>
+      <c r="B13" s="5">
+        <v>6454</v>
+      </c>
+      <c r="C13" s="5" t="inlineStr">
+        <is>
+          <t>5 Paz y Respeto a la Ley</t>
+        </is>
+      </c>
+      <c r="D13" s="5" t="inlineStr">
+        <is>
+          <t>INDICADOR AGLOMERADO 4 HIJA</t>
+        </is>
+      </c>
+      <c r="E13" s="5" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="F13" s="5" t="inlineStr">
+        <is>
+          <t>ACTIVIDAD AGLOMERADO 4 HIJA</t>
+        </is>
+      </c>
+      <c r="G13" s="5" t="inlineStr">
+        <is>
+          <t>Secretaría de Finanzas</t>
         </is>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="0" t="inlineStr">
-        <is>
-          <t>Componente</t>
-        </is>
-      </c>
-      <c r="B14" s="0">
-        <v>5522</v>
-      </c>
-      <c r="C14" s="0" t="inlineStr">
-        <is>
-          <t>1 Salud y Vida Digna</t>
-        </is>
-      </c>
-      <c r="D14" s="0" t="inlineStr">
-        <is>
-          <t>Calificación crediticia de la Entidad</t>
-        </is>
-      </c>
-      <c r="F14" s="0" t="inlineStr">
-        <is>
-          <t>Supuesto</t>
-        </is>
-      </c>
-      <c r="G14" s="0" t="inlineStr">
+      <c r="A14" s="5" t="inlineStr">
+        <is>
+          <t>Fin</t>
+        </is>
+      </c>
+      <c r="B14" s="5">
+        <v>6457</v>
+      </c>
+      <c r="C14" s="5" t="inlineStr">
+        <is>
+          <t>1.2 Aumento en el bienestar y la calidad de vida de la población del estado.</t>
+        </is>
+      </c>
+      <c r="D14" s="5" t="inlineStr">
+        <is>
+          <t>INDICADOR AGLOMERADO PADRE 5 | INDICADOR AGLOMERADO PADRE 5 2</t>
+        </is>
+      </c>
+      <c r="E14" s="5" t="inlineStr">
+        <is>
+          <t>MEDIO PADRE | AA</t>
+        </is>
+      </c>
+      <c r="F14" s="5" t="inlineStr">
+        <is>
+          <t>ACTIVIDAD AGLOMERADO 5 PADRE</t>
+        </is>
+      </c>
+      <c r="G14" s="5" t="inlineStr">
         <is>
           <t>Secretaría de Finanzas</t>
         </is>
@@ -327,30 +344,31 @@
     <row r="15" spans="1:7">
       <c r="A15" s="0" t="inlineStr">
         <is>
-          <t>Actividad</t>
+          <t>Fin</t>
         </is>
       </c>
       <c r="B15" s="0">
-        <v>5529</v>
+        <v>6457</v>
       </c>
       <c r="C15" s="0" t="inlineStr">
         <is>
-          <t>2 Educación, Cultura y Deporte</t>
-        </is>
-      </c>
-      <c r="D15" s="0" t="inlineStr">
-        <is>
-          <t>Monto de los recursos subastados a través del Portal web público TEST</t>
+          <t>1.2 Aumento en el bienestar y la calidad de vida de la población del estado.</t>
+        </is>
+      </c>
+      <c r="D15" s="3" t="inlineStr">
+        <is>
+          <t>ACTIVIDAD AGLOMERADO 5 HIJA 2
+</t>
         </is>
       </c>
       <c r="E15" s="0" t="inlineStr">
         <is>
-          <t>123</t>
+          <t>A</t>
         </is>
       </c>
       <c r="F15" s="0" t="inlineStr">
         <is>
-          <t>Aprovechar los recursos propios</t>
+          <t>ACTIVIDAD AGLOMERADO 5 PADRE</t>
         </is>
       </c>
       <c r="G15" s="0" t="inlineStr">
@@ -375,12 +393,12 @@
       </c>
       <c r="D16" s="0" t="inlineStr">
         <is>
-          <t>INDICADOR AGLOMERADO PADRE 5</t>
+          <t>INDICADOR AGLOMERADO HIJA 2</t>
         </is>
       </c>
       <c r="E16" s="0" t="inlineStr">
         <is>
-          <t>MEDIO PADRE</t>
+          <t>A</t>
         </is>
       </c>
       <c r="F16" s="0" t="inlineStr">
@@ -395,36 +413,35 @@
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="0" t="inlineStr">
+      <c r="A17" s="5" t="inlineStr">
         <is>
           <t>Fin</t>
         </is>
       </c>
-      <c r="B17" s="0">
-        <v>6458</v>
-      </c>
-      <c r="C17" s="0" t="inlineStr">
-        <is>
-          <t>1.2 Aumento en el bienestar y la calidad de vida de la población del estado.</t>
-        </is>
-      </c>
-      <c r="D17" s="3" t="inlineStr">
-        <is>
-          <t>ACTIVIDAD AGLOMERADO 5 HIJA 2
-</t>
-        </is>
-      </c>
-      <c r="E17" s="0" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="F17" s="0" t="inlineStr">
-        <is>
-          <t>ACTIVIDAD AGLOMERADO 5 HIJA</t>
-        </is>
-      </c>
-      <c r="G17" s="0" t="inlineStr">
+      <c r="B17" s="5">
+        <v>6459</v>
+      </c>
+      <c r="C17" s="5" t="inlineStr">
+        <is>
+          <t>6 Gobierno Ciudadano</t>
+        </is>
+      </c>
+      <c r="D17" s="5" t="inlineStr">
+        <is>
+          <t>INDICADOR PADRE 6</t>
+        </is>
+      </c>
+      <c r="E17" s="5" t="inlineStr">
+        <is>
+          <t>423</t>
+        </is>
+      </c>
+      <c r="F17" s="5" t="inlineStr">
+        <is>
+          <t>ACTIVIDAD AGLOMERADO 6 PADRE</t>
+        </is>
+      </c>
+      <c r="G17" s="5" t="inlineStr">
         <is>
           <t>Secretaría de Finanzas</t>
         </is>
@@ -433,70 +450,70 @@
     <row r="18" spans="1:7">
       <c r="A18" s="0" t="inlineStr">
         <is>
+          <t>Fin</t>
+        </is>
+      </c>
+      <c r="B18" s="0">
+        <v>6459</v>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>6 Gobierno Ciudadano</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>INDICADOR HIJA 6</t>
+        </is>
+      </c>
+      <c r="E18" s="0" t="inlineStr">
+        <is>
+          <t>MEDIO HIJA</t>
+        </is>
+      </c>
+      <c r="F18" s="0" t="inlineStr">
+        <is>
+          <t>ACTIVIDAD AGLOMERADO 6 PADRE</t>
+        </is>
+      </c>
+      <c r="G18" s="0" t="inlineStr">
+        <is>
+          <t>Secretaría de Finanzas</t>
+        </is>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="5" t="inlineStr">
+        <is>
           <t>Actividad</t>
         </is>
       </c>
-      <c r="B18" s="0">
+      <c r="B19" s="5">
         <v>6461</v>
       </c>
-      <c r="C18" s="0" t="inlineStr">
+      <c r="C19" s="5" t="inlineStr">
         <is>
           <t>1.1 Ampliación e incremento del acceso a los servicios de salud para la ciudadanía. </t>
         </is>
       </c>
-      <c r="D18" s="0" t="inlineStr">
+      <c r="D19" s="5" t="inlineStr">
         <is>
           <t>Indicador 7 padre</t>
         </is>
       </c>
-      <c r="E18" s="0" t="inlineStr">
+      <c r="E19" s="5" t="inlineStr">
         <is>
           <t>eqwe</t>
         </is>
       </c>
-      <c r="F18" s="0" t="inlineStr">
+      <c r="F19" s="5" t="inlineStr">
         <is>
           <t>ACTIVIDAD AGLOMERADO 7 PADRE</t>
         </is>
       </c>
-      <c r="G18" s="0" t="inlineStr">
-        <is>
-          <t>Secretaría de Finanzas</t>
-        </is>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="0" t="inlineStr">
-        <is>
-          <t>Actividad</t>
-        </is>
-      </c>
-      <c r="B19" s="0">
-        <v>5889</v>
-      </c>
-      <c r="C19" s="0" t="inlineStr">
-        <is>
-          <t>6.1.1.1 Fortalecer la transparencia institucional y el acceso a la información.</t>
-        </is>
-      </c>
-      <c r="D19" s="0" t="inlineStr">
-        <is>
-          <t>Porcentaje de supervisiones realizadas con respecto al total de supervisiones programadas para los Órganos Internos de Control</t>
-        </is>
-      </c>
-      <c r="E19" s="0" t="inlineStr">
-        <is>
-          <t>Minutas de trabajo de las Supervisiones realizadas a los Órganos Internos de Control</t>
-        </is>
-      </c>
-      <c r="F19" s="0" t="inlineStr">
-        <is>
-          <t>Los Órganos Internos  de Control entregan la información y soportes documentales para la Supervisión.</t>
-        </is>
-      </c>
-      <c r="G19" s="0" t="inlineStr">
-        <is>
-          <t>Secretaría de la Contraloría</t>
+      <c r="G19" s="5" t="inlineStr">
+        <is>
+          <t>Secretaría de Finanzas</t>
         </is>
       </c>
     </row>
@@ -507,31 +524,198 @@
         </is>
       </c>
       <c r="B20" s="0">
-        <v>5893</v>
+        <v>6461</v>
       </c>
       <c r="C20" s="0" t="inlineStr">
         <is>
-          <t>6.1.1.1 Fortalecer la transparencia institucional y el acceso a la información.</t>
+          <t>1.1 Ampliación e incremento del acceso a los servicios de salud para la ciudadanía. </t>
         </is>
       </c>
       <c r="D20" s="0" t="inlineStr">
         <is>
-          <t>Porcentaje de servidores públicos del Poder Ejecutivo que presentaron su declaración de inicio y/o conclusión en tiempo y forma, con respecto al total de servidores públicos obligados</t>
+          <t>AGLOMERADO 7 HIJA</t>
         </is>
       </c>
       <c r="E20" s="0" t="inlineStr">
         <is>
-          <t>Aplicación WEB SEMOD (Seguimiento de movimientos y declaraciones) y Padrón de Servidores Públicos Obligados</t>
+          <t>aaa</t>
         </is>
       </c>
       <c r="F20" s="0" t="inlineStr">
         <is>
-          <t>Los servidores públicos del Poder Ejecutivo del Estado de Querétaro conocen la obligación de dar cumplimiento a la presentación de la declaración de modificación de situación patrimonial y de interés de inicio y/o conclusión, así como la fecha límite de presentación. El sistema informático para la presentación de la declaración de modificación de situación patrimonial y de intereses, tiene las condiciones tecnológicas cubiertas. </t>
+          <t>ACTIVIDAD AGLOMERADO 7 PADRE</t>
         </is>
       </c>
       <c r="G20" s="0" t="inlineStr">
         <is>
-          <t>Secretaría de la Contraloría</t>
+          <t>Secretaría de Finanzas</t>
+        </is>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="0" t="inlineStr">
+        <is>
+          <t>Actividad</t>
+        </is>
+      </c>
+      <c r="B21" s="0">
+        <v>6461</v>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>1.1 Ampliación e incremento del acceso a los servicios de salud para la ciudadanía. </t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>AGLOMERADO 7 HIJA 2</t>
+        </is>
+      </c>
+      <c r="E21" s="0" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="F21" s="0" t="inlineStr">
+        <is>
+          <t>ACTIVIDAD AGLOMERADO 7 PADRE</t>
+        </is>
+      </c>
+      <c r="G21" s="0" t="inlineStr">
+        <is>
+          <t>Secretaría de Finanzas</t>
+        </is>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="5" t="inlineStr">
+        <is>
+          <t>Actividad</t>
+        </is>
+      </c>
+      <c r="B22" s="5">
+        <v>5529</v>
+      </c>
+      <c r="C22" s="5" t="inlineStr">
+        <is>
+          <t>2 Educación, Cultura y Deporte</t>
+        </is>
+      </c>
+      <c r="D22" s="5" t="inlineStr">
+        <is>
+          <t>Monto de los recursos subastados a través del Portal web público TEST | Monto de los recursos subastados a través del Portal web público TEST | Monto de los recursos subastados a través del Portal web público TEST</t>
+        </is>
+      </c>
+      <c r="E22" s="5" t="inlineStr">
+        <is>
+          <t>123 | 123 | 123</t>
+        </is>
+      </c>
+      <c r="F22" s="5" t="inlineStr">
+        <is>
+          <t>Aprovechar los recursos propios</t>
+        </is>
+      </c>
+      <c r="G22" s="5" t="inlineStr">
+        <is>
+          <t>Secretaría de Finanzas</t>
+        </is>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="5" t="inlineStr">
+        <is>
+          <t>Componente</t>
+        </is>
+      </c>
+      <c r="B23" s="5">
+        <v>6450</v>
+      </c>
+      <c r="C23" s="5" t="inlineStr">
+        <is>
+          <t>1.1.2 Consolidar el sistema de salud con apoyo interinstitucional</t>
+        </is>
+      </c>
+      <c r="D23" s="5" t="inlineStr">
+        <is>
+          <t>Prueba Acumulativo | Prueba Acumulativo | Prueba Acumulativo | Prueba Acumulativo | Prueba Acumulativo | Prueba Acumulativo</t>
+        </is>
+      </c>
+      <c r="E23" s="5" t="inlineStr">
+        <is>
+          <t>1 | 1 | 1 | 1 | 1 | 1</t>
+        </is>
+      </c>
+      <c r="F23" s="5" t="inlineStr">
+        <is>
+          <t>Actividad Prueba EJE</t>
+        </is>
+      </c>
+      <c r="G23" s="5" t="inlineStr">
+        <is>
+          <t>Secretaría de Finanzas</t>
+        </is>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="5" t="inlineStr">
+        <is>
+          <t>Componente</t>
+        </is>
+      </c>
+      <c r="B24" s="5">
+        <v>6449</v>
+      </c>
+      <c r="C24" s="5" t="inlineStr">
+        <is>
+          <t>1.1.2 Consolidar el sistema de salud con apoyo interinstitucional</t>
+        </is>
+      </c>
+      <c r="D24" s="5" t="inlineStr">
+        <is>
+          <t>Prueba | Prueba | Prueba | Prueba | Prueba | Prueba | Tipo 1 | Tipo 1 | Prueba | Prueba | Prueba | Prueba | Test | Prueba | Test | Prueba | Prueba | Prueba | Prueba | Prueba | Prueba | Prueba | Prueba | Prueba</t>
+        </is>
+      </c>
+      <c r="E24" s="5" t="inlineStr">
+        <is>
+          <t>1 | 1 | 1 | 1 | 1 | 1 | 1 | 1 | 1 | 1 | 1 | 1 | 1 | 1 | 1 | 1 | 1 | 1 | 1 | 1 | 1 | 1 | 1 | 1</t>
+        </is>
+      </c>
+      <c r="F24" s="5" t="inlineStr">
+        <is>
+          <t>Actividad Ejemplo Sin Nada Nuevo</t>
+        </is>
+      </c>
+      <c r="G24" s="5" t="inlineStr">
+        <is>
+          <t>Secretaría de Finanzas</t>
+        </is>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="5" t="inlineStr">
+        <is>
+          <t>Fin</t>
+        </is>
+      </c>
+      <c r="B25" s="5">
+        <v>6451</v>
+      </c>
+      <c r="C25" s="5" t="inlineStr">
+        <is>
+          <t>6 Gobierno Ciudadano</t>
+        </is>
+      </c>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5" t="inlineStr">
+        <is>
+          <t>ACTIVIDAD POA SF</t>
+        </is>
+      </c>
+      <c r="G25" s="5" t="inlineStr">
+        <is>
+          <t>Secretaría de Finanzas</t>
         </is>
       </c>
     </row>

</xml_diff>